<commit_message>
linked well colors to excel pass/fail statuses
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/template.xlsx
+++ b/src/main/resources/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwhite/vCheck1.1/src/main/resources/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{8C3FA340-9985-8B48-A9C6-451B1E02D21A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{60A74CE7-F399-C04F-9B35-9366F264A539}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18460" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   <calcPr calcId="179021"/>
   <customWorkbookViews>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" mergeInterval="0" personalView="1" yWindow="23" windowWidth="923" windowHeight="597" activeSheetId="1"/>
+    <customWorkbookView name="Jill Heath - Personal View" guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1680" windowHeight="927" activeSheetId="1"/>
     <customWorkbookView name="Carrie Andrews - Personal View" guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1"/>
-    <customWorkbookView name="Jill Heath - Personal View" guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1680" windowHeight="927" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2011,7 +2011,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{379B1AED-9713-5643-9AE1-ABD20A6A019C}" diskRevisions="1" revisionId="31" version="4" preserveHistory="1825">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" diskRevisions="1" revisionId="36" version="5" preserveHistory="1825">
   <header guid="{38C3440D-4EC0-4292-BC84-4A302E87F478}" dateTime="2014-08-25T14:40:29" maxSheetId="5" userName="Nicole VanDyke" r:id="rId12">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -2053,6 +2053,14 @@
     </sheetIdMap>
   </header>
   <header guid="{379B1AED-9713-5643-9AE1-ABD20A6A019C}" dateTime="2018-09-17T15:51:07" maxSheetId="5" userName="Microsoft Office User" r:id="rId17" minRId="29" maxRId="31">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" dateTime="2018-09-17T20:52:05" maxSheetId="5" userName="Microsoft Office User" r:id="rId18" minRId="32" maxRId="36">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2126,8 +2134,42 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="32" sId="1">
+    <nc r="C21">
+      <v>2123</v>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="1">
+    <nc r="C23">
+      <v>12123</v>
+    </nc>
+  </rcc>
+  <rcc rId="34" sId="1">
+    <nc r="C35">
+      <v>12123</v>
+    </nc>
+  </rcc>
+  <rcc rId="35" sId="1">
+    <nc r="C40">
+      <v>123123</v>
+    </nc>
+  </rcc>
+  <rcc rId="36" sId="1">
+    <nc r="C45">
+      <v>123</v>
+    </nc>
+  </rcc>
+  <rcv guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" action="delete"/>
+  <rcv guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" name="Microsoft Office User" id="-296959979" dateTime="2018-09-17T20:51:51"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2455,8 +2497,8 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3171,14 +3213,16 @@
         <f t="array" ref="B21">SUM(IF(A21='Raw Data'!B:B,'Raw Data'!E:E,IF(A21='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>2123</v>
+      </c>
       <c r="D21" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2123</v>
       </c>
       <c r="F21" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3245,14 +3289,16 @@
         <f t="array" ref="B23">SUM(IF(A23='Raw Data'!B:B,'Raw Data'!E:E,IF(A23='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>12123</v>
+      </c>
       <c r="D23" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12123</v>
       </c>
       <c r="F23" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3689,14 +3735,16 @@
         <f t="array" ref="B35">SUM(IF(A35='Raw Data'!B:B,'Raw Data'!E:E,IF(A35='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="5">
+        <v>12123</v>
+      </c>
       <c r="D35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12123</v>
       </c>
       <c r="F35" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3874,14 +3922,16 @@
         <f t="array" ref="B40">SUM(IF(A40='Raw Data'!B:B,'Raw Data'!E:E,IF(A40='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="5">
+        <v>123123</v>
+      </c>
       <c r="D40" s="25" t="str">
         <f t="shared" si="5"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>123123</v>
       </c>
       <c r="F40" s="26" t="e">
         <f t="shared" si="4"/>
@@ -4064,14 +4114,16 @@
         <f t="array" ref="B45">SUM(IF(A45='Raw Data'!B:B,'Raw Data'!E:E,IF(A45='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5">
+        <v>123</v>
+      </c>
       <c r="D45" s="25" t="str">
         <f t="shared" si="5"/>
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="F45" s="26" t="e">
         <f t="shared" si="4"/>
@@ -6067,15 +6119,15 @@
   </protectedRanges>
   <customSheetViews>
     <customSheetView guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" showPageBreaks="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6084,7 +6136,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" showPageBreaks="1">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6897,7 +6949,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6906,7 +6958,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7391,7 +7443,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" topLeftCell="A22">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" topLeftCell="A22">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7399,7 +7451,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" topLeftCell="A22">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" topLeftCell="A22">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -7446,7 +7498,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7454,7 +7506,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
added master control downloader and plate data copy method
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/template.xlsx
+++ b/src/main/resources/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwhite/vCheck1.1/src/main/resources/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{60A74CE7-F399-C04F-9B35-9366F264A539}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{1C94F572-797D-9A4F-AE13-0D6D98DE09A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18460" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   <calcPr calcId="179021"/>
   <customWorkbookViews>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" mergeInterval="0" personalView="1" yWindow="23" windowWidth="923" windowHeight="597" activeSheetId="1"/>
+    <customWorkbookView name="Carrie Andrews - Personal View" guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1"/>
     <customWorkbookView name="Jill Heath - Personal View" guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1680" windowHeight="927" activeSheetId="1"/>
-    <customWorkbookView name="Carrie Andrews - Personal View" guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2011,7 +2011,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" diskRevisions="1" revisionId="36" version="5" preserveHistory="1825">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7475991F-F3DD-AE4C-983D-6AA4356C706B}" diskRevisions="1" revisionId="43" version="6" preserveHistory="1825">
   <header guid="{38C3440D-4EC0-4292-BC84-4A302E87F478}" dateTime="2014-08-25T14:40:29" maxSheetId="5" userName="Nicole VanDyke" r:id="rId12">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -2061,6 +2061,14 @@
     </sheetIdMap>
   </header>
   <header guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" dateTime="2018-09-17T20:52:05" maxSheetId="5" userName="Microsoft Office User" r:id="rId18" minRId="32" maxRId="36">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7475991F-F3DD-AE4C-983D-6AA4356C706B}" dateTime="2018-09-19T11:23:38" maxSheetId="5" userName="Microsoft Office User" r:id="rId19" minRId="37" maxRId="43">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2166,10 +2174,57 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="37" sId="1">
+    <oc r="C35">
+      <v>12123</v>
+    </oc>
+    <nc r="C35"/>
+  </rcc>
+  <rcc rId="38" sId="1">
+    <oc r="C40">
+      <v>123123</v>
+    </oc>
+    <nc r="C40"/>
+  </rcc>
+  <rcc rId="39" sId="1">
+    <oc r="C45">
+      <v>123</v>
+    </oc>
+    <nc r="C45"/>
+  </rcc>
+  <rcc rId="40" sId="1">
+    <oc r="C4">
+      <v>213</v>
+    </oc>
+    <nc r="C4"/>
+  </rcc>
+  <rcc rId="41" sId="1">
+    <oc r="C15">
+      <v>213123</v>
+    </oc>
+    <nc r="C15"/>
+  </rcc>
+  <rcc rId="42" sId="1">
+    <oc r="C21">
+      <v>2123</v>
+    </oc>
+    <nc r="C21"/>
+  </rcc>
+  <rcc rId="43" sId="1">
+    <oc r="C23">
+      <v>12123</v>
+    </oc>
+    <nc r="C23"/>
+  </rcc>
+  <rcv guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" action="delete"/>
+  <rcv guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{5758893F-AFB4-2C4F-8631-297D426C7962}" name="Microsoft Office User" id="-296959979" dateTime="2018-09-17T20:51:51"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2497,8 +2552,8 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2584,16 +2639,14 @@
         <f t="array" ref="B4">SUM(IF(A4='Raw Data'!B:B,'Raw Data'!E:E,IF(A4='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C4" s="12">
-        <v>213</v>
-      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="25" t="str">
         <f t="shared" ref="D4:D35" si="0">IF(AND(C4&lt;=H4,C4&gt;=I4),"PASS","FAIL")</f>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E4" s="11">
         <f>(C4-B4)</f>
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="F4" s="26" t="e">
         <f>E4/B4</f>
@@ -2989,16 +3042,14 @@
         <f t="array" ref="B15">SUM(IF(A15='Raw Data'!B:B,'Raw Data'!E:E,IF(A15='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C15" s="5">
-        <v>213123</v>
-      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" si="3"/>
-        <v>213123</v>
+        <v>0</v>
       </c>
       <c r="F15" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3213,16 +3264,14 @@
         <f t="array" ref="B21">SUM(IF(A21='Raw Data'!B:B,'Raw Data'!E:E,IF(A21='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C21" s="5">
-        <v>2123</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="3"/>
-        <v>2123</v>
+        <v>0</v>
       </c>
       <c r="F21" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3289,16 +3338,14 @@
         <f t="array" ref="B23">SUM(IF(A23='Raw Data'!B:B,'Raw Data'!E:E,IF(A23='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C23" s="5">
-        <v>12123</v>
-      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="3"/>
-        <v>12123</v>
+        <v>0</v>
       </c>
       <c r="F23" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3735,16 +3782,14 @@
         <f t="array" ref="B35">SUM(IF(A35='Raw Data'!B:B,'Raw Data'!E:E,IF(A35='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C35" s="5">
-        <v>12123</v>
-      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E35" s="11">
         <f t="shared" si="3"/>
-        <v>12123</v>
+        <v>0</v>
       </c>
       <c r="F35" s="26" t="e">
         <f t="shared" si="4"/>
@@ -3922,16 +3967,14 @@
         <f t="array" ref="B40">SUM(IF(A40='Raw Data'!B:B,'Raw Data'!E:E,IF(A40='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C40" s="5">
-        <v>123123</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="25" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="3"/>
-        <v>123123</v>
+        <v>0</v>
       </c>
       <c r="F40" s="26" t="e">
         <f t="shared" si="4"/>
@@ -4114,16 +4157,14 @@
         <f t="array" ref="B45">SUM(IF(A45='Raw Data'!B:B,'Raw Data'!E:E,IF(A45='Raw Data'!A:A,'Raw Data'!D:D,0)))</f>
         <v>0</v>
       </c>
-      <c r="C45" s="5">
-        <v>123</v>
-      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="25" t="str">
         <f t="shared" si="5"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="F45" s="26" t="e">
         <f t="shared" si="4"/>
@@ -6119,15 +6160,15 @@
   </protectedRanges>
   <customSheetViews>
     <customSheetView guid="{D6E20411-6DF8-1745-A20C-51C951CD7C61}">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C23"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" showPageBreaks="1">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6136,7 +6177,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" showPageBreaks="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6949,7 +6990,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6958,7 +6999,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7443,7 +7484,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" topLeftCell="A22">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" topLeftCell="A22">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7451,7 +7492,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" topLeftCell="A22">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}" topLeftCell="A22">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -7498,7 +7539,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
+    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7506,7 +7547,7 @@
         <oddFooter>&amp;LHPF-112 REV02</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}">
+    <customSheetView guid="{D4BC0202-85EA-4C8E-ACF5-B79344380D31}">
       <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
button style edits and funciton
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/template.xlsx
+++ b/src/main/resources/assets/template.xlsx
@@ -2010,6 +2010,88 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B1BC44F1-0229-4768-9F52-A9155E5C8747}" diskRevisions="1" revisionId="27" version="2" preserveHistory="1825">
+  <header guid="{87E6FDFD-96EF-4286-BAB0-CE840E5BB314}" dateTime="2013-05-09T14:17:33" maxSheetId="4" userName="HPF-WS-02" r:id="rId1">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{92ED58A7-547D-43F9-A53A-E1DBCD9413CF}" dateTime="2013-05-09T14:20:29" maxSheetId="4" userName="HPF-WS-02" r:id="rId2" minRId="1">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3284D0FD-EAB3-451D-A1EA-1F3996093AD3}" dateTime="2013-05-09T14:21:00" maxSheetId="4" userName="HPF-WS-02" r:id="rId3" minRId="2">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6A8566BC-BEFC-4993-83CF-C26E96020A53}" dateTime="2013-05-09T14:22:07" maxSheetId="4" userName="HPF-WS-02" r:id="rId4" minRId="3" maxRId="4">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{46DB9F3D-406A-4254-95DE-45DFAE09C1D7}" dateTime="2013-05-09T14:25:28" maxSheetId="4" userName="Curt Franklin" r:id="rId5">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4006E6F5-B5B6-4F9A-819F-A1B6CA35E69E}" dateTime="2013-05-09T14:25:59" maxSheetId="4" userName="Curt Franklin" r:id="rId6" minRId="5" maxRId="6">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D248C0D1-3374-4C24-8439-C5C338305024}" dateTime="2013-05-09T14:26:18" maxSheetId="4" userName="Curt Franklin" r:id="rId7">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{93BA7A30-01AA-4DA2-8D44-8764B57E57AA}" dateTime="2013-05-09T15:45:06" maxSheetId="4" userName="HPF-WS-02" r:id="rId8">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{97BA56BD-24AA-4D3B-B231-F88B4C6D364F}" dateTime="2013-05-09T15:51:02" maxSheetId="4" userName="HPF-WS-02" r:id="rId9" minRId="7" maxRId="26">
+    <sheetIdMap count="3">
+      <sheetId val="0"/>
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7B051AFF-644B-4C77-A8FA-1AEAF75967F4}" dateTime="2013-05-09T16:03:06" maxSheetId="5" userName="Nicole VanDyke" r:id="rId10" minRId="27">
+    <sheetIdMap count="4">
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+      <sheetId val="65535"/>
+      <sheetId val="6911"/>
+    </sheetIdMap>
+    <reviewedList count="1">
+      <reviewed rId="27"/>
+    </reviewedList>
+  </header>
+  <header guid="{F6B53A00-50BB-4E43-834F-0A964A96FE66}" dateTime="2013-05-09T16:03:19" maxSheetId="5" userName="Nicole VanDyke" r:id="rId11">
+    <sheetIdMap count="4">
+      <sheetId val="32"/>
+      <sheetId val="0"/>
+      <sheetId val="65535"/>
+      <sheetId val="14848"/>
+    </sheetIdMap>
+  </header>
   <header guid="{38C3440D-4EC0-4292-BC84-4A302E87F478}" dateTime="2014-08-25T14:40:29" maxSheetId="5" userName="Nicole VanDyke" r:id="rId12">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -2045,6 +2127,24 @@
 </headers>
 </file>
 
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="27" sheetId="4" name="[HPF-xxx Backend Volume Check Template.xls]Sheet1" sheetPosition="3"/>
+  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="delete"/>
+  <rcv guid="{9F84A064-4324-4DEF-94DB-E2DBDFD7C916}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="delete"/>
@@ -2071,6 +2171,252 @@
 <file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{A079EE5E-548E-44E6-8CD6-9DE38EF18C5D}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>audit test</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="2" sId="1">
+    <oc r="B1" t="inlineStr">
+      <is>
+        <t>audit test</t>
+      </is>
+    </oc>
+    <nc r="B1"/>
+  </rcc>
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="3" sId="3">
+    <nc r="C27" t="inlineStr">
+      <is>
+        <t>Golda Monohon</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" sId="3" numFmtId="19">
+    <nc r="E27">
+      <v>41403</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="5" sId="3">
+    <nc r="C29" t="inlineStr">
+      <is>
+        <t>Curt Franklin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="3" odxf="1" dxf="1" numFmtId="19">
+    <nc r="E29">
+      <v>41403</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="delete"/>
+  <rcv guid="{E305E553-7664-4FB6-A7EB-4038600BBB9A}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="delete"/>
+  <rcv guid="{0FE0FB27-0CB1-41B7-8EAA-ED1EF06EC50A}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="7" sId="3">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="8" sId="3">
+    <nc r="F12" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="3">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="10" sId="3">
+    <nc r="F13" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="3">
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="3">
+    <nc r="F14" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="3">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="3">
+    <nc r="F15" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="3">
+    <nc r="E16" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="3">
+    <nc r="F16" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="3">
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="3">
+    <nc r="F17" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="3">
+    <nc r="E21" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" sId="3">
+    <nc r="F21" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="3">
+    <nc r="E18" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="3">
+    <nc r="F18" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="23" sId="3">
+    <nc r="E22" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="24" sId="3">
+    <nc r="F22" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" sId="3">
+    <nc r="E25" t="inlineStr">
+      <is>
+        <t>Pass</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="3" odxf="1" dxf="1">
+    <nc r="F25" t="inlineStr">
+      <is>
+        <t>GLM  5/9/2013</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <b val="0"/>
+        <sz val="9"/>
+      </font>
+    </odxf>
+    <ndxf>
+      <font>
+        <b/>
+        <sz val="9"/>
+      </font>
+    </ndxf>
+  </rcc>
 </revisions>
 </file>
 

</xml_diff>

<commit_message>
changed default import directory and how the update method works
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/template.xlsx
+++ b/src/main/resources/assets/template.xlsx
@@ -2421,7 +2421,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{B1BC44F1-0229-4768-9F52-A9155E5C8747}" name="Microsoft Office User" id="-296946436" dateTime="2018-10-09T13:27:14"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>